<commit_message>
#73 Update the normalization
</commit_message>
<xml_diff>
--- a/plantFloorManager/SQL_Database/Dataset02_v1.xlsx
+++ b/plantFloorManager/SQL_Database/Dataset02_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myisepipp-my.sharepoint.com/personal/1230948_isep_ipp_pt/Documents/Ficheiros de Conversa do Microsoft Teams/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://0cms6-my.sharepoint.com/personal/diogopereira_0cms6_onmicrosoft_com/Documents/Faculdade/Código 2º Ano/sem3-pi-2024-g094/plantFloorManager/SQL_Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="522" documentId="8_{61104BE5-191E-4C22-96ED-F0E59940F269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E9944C0-C062-43B4-9771-F47BB3D6AB02}"/>
+  <xr:revisionPtr revIDLastSave="537" documentId="8_{61104BE5-191E-4C22-96ED-F0E59940F269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4B7044A-91C7-42CA-8859-DA48977632B5}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" firstSheet="6" activeTab="7" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="6" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -1123,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15D9EF7-7F05-4929-9267-83A028A1D45D}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B19"/>
+      <selection activeCell="B14" sqref="B14:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1250,44 +1250,8 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B13" t="str">
-        <f>_xlfn.CONCAT("insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID) values ('",A2,"', '",B2,"', '",C2,"', 1, ",D2,");")</f>
-        <v>insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID) values ('AS12945T22', 'La Belle 22 5l pot', '5l 22 cm aluminium and teflon non stick pot', 1, 130);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B14" t="str">
-        <f t="shared" ref="B14:B19" si="0">_xlfn.CONCAT("insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID) values ('",A3,"', '",B3,"', '",C3,"', 1, ",D3,");")</f>
-        <v>insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID) values ('AS12945S22', 'Pro 22 5l pot', '5l 22 cm stainless steel pot', 1, 125);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID) values ('AS12945S20', 'Pro 20 3l pot', '3l 20 cm stainless steel pot', 1, 125);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID) values ('AS12945S17', 'Pro 17 2l pot', '2l 17 cm stainless steel pot', 1, 125);</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID) values ('AS12945P17', 'Pro 17 2l sauce pan', '2l 17 cm stainless steel souce pan', 1, 132);</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID) values ('AS12945S48', 'Pro 17 lid', '17 cm stainless steel lid', 1, 145);</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID) values ('AS12945G48', 'Pro Clear 17 lid', '17 cm glass lid', 1, 146);</v>
+        <f>_xlfn.CONCAT("insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID, Part_ID) values ('",A2,"', '",B2,"', '",C2,"', 1, ",D2,");")</f>
+        <v>insert into Product (Product_ID, Product_Name, Product_Description, Factory_Plant_ID, Family_ID, Part_ID) values ('AS12945T22', 'La Belle 22 5l pot', '5l 22 cm aluminium and teflon non stick pot', 1, 130);</v>
       </c>
     </row>
   </sheetData>
@@ -1302,7 +1266,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1396,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE470C24-4865-4CED-BECB-9AD0BD718C1F}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1409,7 +1373,7 @@
     <col min="6" max="6" width="14.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -1429,7 +1393,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1448,8 +1412,12 @@
       <c r="F2" s="1">
         <v>45558</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT("insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (",A2,", '",C2,"', ",D2,");")</f>
+        <v>insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (1, 'AS12945S22', 5);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1468,8 +1436,12 @@
       <c r="F3" s="1">
         <v>45558</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H10" si="0">_xlfn.CONCAT("insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (",A3,", '",C3,"', ",D3,");")</f>
+        <v>insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (1, 'AS12945S20', 15);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1488,8 +1460,12 @@
       <c r="F4" s="1">
         <v>45560</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (2, 'AS12945S22', 10);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1508,8 +1484,12 @@
       <c r="F5" s="1">
         <v>45560</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (3, 'AS12945S22', 10);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1528,8 +1508,12 @@
       <c r="F6" s="1">
         <v>45560</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (3, 'AS12945S20', 10);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1548,8 +1532,12 @@
       <c r="F7" s="1">
         <v>45560</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (4, 'AS12945S22', 4);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1568,8 +1556,12 @@
       <c r="F8" s="1">
         <v>45560</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (5, 'AS12945S22', 12);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1588,8 +1580,12 @@
       <c r="F9" s="1">
         <v>45561</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (6, 'AS12945S17', 8);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1607,6 +1603,10 @@
       </c>
       <c r="F10" s="1">
         <v>45561</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Customer_Order_Product(Customer_Order_ID, Product_ID, Quantity) values (7, 'AS12945S22', 7);</v>
       </c>
     </row>
   </sheetData>
@@ -1946,7 +1946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1118E112-BCDE-455B-843A-6C293EDE0CEE}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -2274,7 +2274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D833FD3A-319E-497B-BBC6-9FC6F2F78F3D}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" t="str">
-        <f t="shared" ref="B43:B60" si="2">_xlfn.CONCAT("insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('",A3,"', '",B3,"', ",D3,");")</f>
+        <f t="shared" ref="B44:B60" si="2">_xlfn.CONCAT("insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('",A3,"', '",B3,"', ",D3,");")</f>
         <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S22', 'PN52384R50', 1);</v>
       </c>
     </row>

</xml_diff>